<commit_message>
Adicionou arquivos de input/output
</commit_message>
<xml_diff>
--- a/notas.xlsx
+++ b/notas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH52"/>
+  <dimension ref="A1:AH53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -826,7 +826,7 @@
         <v>0.2</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -874,10 +874,10 @@
         <v>0</v>
       </c>
       <c r="S4" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="T4" t="n">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="U4" t="n">
         <v>0.3333333333333333</v>
@@ -904,19 +904,19 @@
         <v>0</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.625</v>
+        <v>0.25</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.8571428571428571</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="AE4" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AF4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG4" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AH4" t="inlineStr">
         <is>
@@ -5571,29 +5571,29 @@
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>211063004</t>
+          <t>211062992</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="C48" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E48" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F48" t="n">
         <v>0</v>
       </c>
       <c r="G48" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="H48" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="I48" t="n">
         <v>0</v>
@@ -5617,16 +5617,16 @@
         <v>0</v>
       </c>
       <c r="P48" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="Q48" t="n">
-        <v>0.1428571428571428</v>
+        <v>0</v>
       </c>
       <c r="R48" t="n">
         <v>0</v>
       </c>
       <c r="S48" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="T48" t="n">
         <v>0</v>
@@ -5635,10 +5635,10 @@
         <v>0</v>
       </c>
       <c r="V48" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="W48" t="n">
-        <v>0.3333333333333333</v>
+        <v>0</v>
       </c>
       <c r="X48" t="n">
         <v>0</v>
@@ -5668,7 +5668,7 @@
         <v>0</v>
       </c>
       <c r="AG48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH48" t="inlineStr">
         <is>
@@ -5679,35 +5679,35 @@
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>211063149</t>
+          <t>211063004</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="C49" t="n">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="D49" t="n">
         <v>1</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="F49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G49" t="n">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="H49" t="n">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="I49" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K49" t="n">
         <v>0</v>
@@ -5725,34 +5725,34 @@
         <v>0</v>
       </c>
       <c r="P49" t="n">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="Q49" t="n">
-        <v>1</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="R49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S49" t="n">
-        <v>0.875</v>
+        <v>0.25</v>
       </c>
       <c r="T49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V49" t="n">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="W49" t="n">
-        <v>1</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="X49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z49" t="n">
         <v>0</v>
@@ -5764,40 +5764,40 @@
         <v>0</v>
       </c>
       <c r="AC49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG49" t="n">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="AH49" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>II</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>211063158</t>
+          <t>211063149</t>
         </is>
       </c>
       <c r="B50" t="n">
         <v>1</v>
       </c>
       <c r="C50" t="n">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
       <c r="D50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E50" t="n">
         <v>1</v>
@@ -5818,7 +5818,7 @@
         <v>1</v>
       </c>
       <c r="K50" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L50" t="n">
         <v>0</v>
@@ -5848,7 +5848,7 @@
         <v>1</v>
       </c>
       <c r="U50" t="n">
-        <v>0.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="V50" t="n">
         <v>1</v>
@@ -5884,7 +5884,7 @@
         <v>1</v>
       </c>
       <c r="AG50" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="AH50" t="inlineStr">
         <is>
@@ -5895,23 +5895,23 @@
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>211063185</t>
+          <t>211063158</t>
         </is>
       </c>
       <c r="B51" t="n">
         <v>1</v>
       </c>
       <c r="C51" t="n">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="D51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E51" t="n">
         <v>1</v>
       </c>
       <c r="F51" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="G51" t="n">
         <v>1</v>
@@ -5956,10 +5956,10 @@
         <v>1</v>
       </c>
       <c r="U51" t="n">
-        <v>1</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="V51" t="n">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="W51" t="n">
         <v>1</v>
@@ -6003,14 +6003,14 @@
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>211063194</t>
+          <t>211063185</t>
         </is>
       </c>
       <c r="B52" t="n">
         <v>1</v>
       </c>
       <c r="C52" t="n">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="D52" t="n">
         <v>1</v>
@@ -6028,7 +6028,7 @@
         <v>2</v>
       </c>
       <c r="I52" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J52" t="n">
         <v>1</v>
@@ -6067,7 +6067,7 @@
         <v>1</v>
       </c>
       <c r="V52" t="n">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="W52" t="n">
         <v>1</v>
@@ -6105,6 +6105,114 @@
       <c r="AH52" t="inlineStr">
         <is>
           <t>MS</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>211063194</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>1</v>
+      </c>
+      <c r="C53" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="D53" t="n">
+        <v>1</v>
+      </c>
+      <c r="E53" t="n">
+        <v>1</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="G53" t="n">
+        <v>1</v>
+      </c>
+      <c r="H53" t="n">
+        <v>2</v>
+      </c>
+      <c r="I53" t="n">
+        <v>1</v>
+      </c>
+      <c r="J53" t="n">
+        <v>1</v>
+      </c>
+      <c r="K53" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L53" t="n">
+        <v>2</v>
+      </c>
+      <c r="M53" t="n">
+        <v>1</v>
+      </c>
+      <c r="N53" t="n">
+        <v>1</v>
+      </c>
+      <c r="O53" t="n">
+        <v>0</v>
+      </c>
+      <c r="P53" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q53" t="n">
+        <v>1</v>
+      </c>
+      <c r="R53" t="n">
+        <v>1</v>
+      </c>
+      <c r="S53" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="T53" t="n">
+        <v>1</v>
+      </c>
+      <c r="U53" t="n">
+        <v>1</v>
+      </c>
+      <c r="V53" t="n">
+        <v>1</v>
+      </c>
+      <c r="W53" t="n">
+        <v>1</v>
+      </c>
+      <c r="X53" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y53" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z53" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA53" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB53" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC53" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD53" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE53" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF53" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG53" t="n">
+        <v>25</v>
+      </c>
+      <c r="AH53" t="inlineStr">
+        <is>
+          <t>SS</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Algumas correções de notas
</commit_message>
<xml_diff>
--- a/notas.xlsx
+++ b/notas.xlsx
@@ -823,7 +823,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -832,13 +832,13 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="H4" t="n">
         <v>1</v>
@@ -871,25 +871,25 @@
         <v>0.7142857142857143</v>
       </c>
       <c r="R4" t="n">
-        <v>0</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="S4" t="n">
         <v>0</v>
       </c>
       <c r="T4" t="n">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="U4" t="n">
-        <v>0.3333333333333333</v>
+        <v>0</v>
       </c>
       <c r="V4" t="n">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="W4" t="n">
         <v>0</v>
       </c>
       <c r="X4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y4" t="n">
         <v>0</v>
@@ -916,7 +916,7 @@
         <v>0</v>
       </c>
       <c r="AG4" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AH4" t="inlineStr">
         <is>
@@ -3523,28 +3523,28 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="C29" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D29" t="n">
         <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="G29" t="n">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="H29" t="n">
         <v>1</v>
       </c>
       <c r="I29" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J29" t="n">
         <v>1</v>
@@ -3571,25 +3571,25 @@
         <v>0.2857142857142857</v>
       </c>
       <c r="R29" t="n">
-        <v>0.2857142857142857</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="S29" t="n">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="T29" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="U29" t="n">
         <v>0</v>
       </c>
       <c r="V29" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="W29" t="n">
-        <v>0.6666666666666666</v>
+        <v>0</v>
       </c>
       <c r="X29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y29" t="n">
         <v>0</v>
@@ -3616,7 +3616,7 @@
         <v>1</v>
       </c>
       <c r="AG29" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="AH29" t="inlineStr">
         <is>
@@ -4927,10 +4927,10 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="C42" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D42" t="n">
         <v>0</v>
@@ -4975,25 +4975,25 @@
         <v>1</v>
       </c>
       <c r="R42" t="n">
-        <v>0.5714285714285714</v>
+        <v>1</v>
       </c>
       <c r="S42" t="n">
-        <v>0.625</v>
+        <v>0</v>
       </c>
       <c r="T42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U42" t="n">
-        <v>0.3333333333333333</v>
+        <v>0</v>
       </c>
       <c r="V42" t="n">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="W42" t="n">
-        <v>0.6666666666666666</v>
+        <v>0</v>
       </c>
       <c r="X42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y42" t="n">
         <v>0</v>
@@ -5020,11 +5020,11 @@
         <v>1</v>
       </c>
       <c r="AG42" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="AH42" t="inlineStr">
         <is>
-          <t>MI</t>
+          <t>MM</t>
         </is>
       </c>
     </row>

</xml_diff>